<commit_message>
retaking the project from the SNARK, upgrading all files
</commit_message>
<xml_diff>
--- a/Growth/TTR_GrowthParameters.xlsx
+++ b/Growth/TTR_GrowthParameters.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="600" yWindow="120" windowWidth="11715" windowHeight="6975"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="growth models" sheetId="1" r:id="rId1"/>
+    <sheet name="Pred vb" sheetId="2" r:id="rId2"/>
+    <sheet name="age" sheetId="4" r:id="rId3"/>
+    <sheet name="allage" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t>Bottlenose dolphin (Tursiops truncatus)</t>
   </si>
@@ -52,6 +53,159 @@
   </si>
   <si>
     <t>length ~ Linf*exp(-K*exp(-age*to))</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>len</t>
+  </si>
+  <si>
+    <t>age0</t>
+  </si>
+  <si>
+    <t>age1</t>
+  </si>
+  <si>
+    <t>age2</t>
+  </si>
+  <si>
+    <t>age3</t>
+  </si>
+  <si>
+    <t>age4</t>
+  </si>
+  <si>
+    <t>age5</t>
+  </si>
+  <si>
+    <t>age6</t>
+  </si>
+  <si>
+    <t>age7</t>
+  </si>
+  <si>
+    <t>age8</t>
+  </si>
+  <si>
+    <t>age9</t>
+  </si>
+  <si>
+    <t>age10</t>
+  </si>
+  <si>
+    <t>age11</t>
+  </si>
+  <si>
+    <t>age12</t>
+  </si>
+  <si>
+    <t>age13</t>
+  </si>
+  <si>
+    <t>age14</t>
+  </si>
+  <si>
+    <t>age15</t>
+  </si>
+  <si>
+    <t>age16</t>
+  </si>
+  <si>
+    <t>age17</t>
+  </si>
+  <si>
+    <t>age18</t>
+  </si>
+  <si>
+    <t>age19</t>
+  </si>
+  <si>
+    <t>age20</t>
+  </si>
+  <si>
+    <t>age21</t>
+  </si>
+  <si>
+    <t>age22</t>
+  </si>
+  <si>
+    <t>age23</t>
+  </si>
+  <si>
+    <t>age24</t>
+  </si>
+  <si>
+    <t>age25</t>
+  </si>
+  <si>
+    <t>age26</t>
+  </si>
+  <si>
+    <t>age27</t>
+  </si>
+  <si>
+    <t>age28</t>
+  </si>
+  <si>
+    <t>age29</t>
+  </si>
+  <si>
+    <t>age30</t>
+  </si>
+  <si>
+    <t>age31</t>
+  </si>
+  <si>
+    <t>age32</t>
+  </si>
+  <si>
+    <t>age33</t>
+  </si>
+  <si>
+    <t>age34</t>
+  </si>
+  <si>
+    <t>age35</t>
+  </si>
+  <si>
+    <t>age36</t>
+  </si>
+  <si>
+    <t>age37</t>
+  </si>
+  <si>
+    <t>age38</t>
+  </si>
+  <si>
+    <t>age39</t>
+  </si>
+  <si>
+    <t>age40</t>
+  </si>
+  <si>
+    <t>age41</t>
+  </si>
+  <si>
+    <t>age42</t>
+  </si>
+  <si>
+    <t>age43</t>
+  </si>
+  <si>
+    <t>age44</t>
+  </si>
+  <si>
+    <t>age45</t>
+  </si>
+  <si>
+    <t>age46</t>
+  </si>
+  <si>
+    <t>age47</t>
+  </si>
+  <si>
+    <t>allages</t>
   </si>
 </sst>
 </file>
@@ -87,8 +241,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,7 +541,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -459,7 +614,7 @@
         <v>0.22274579999999999</v>
       </c>
       <c r="D9">
-        <v>4.4724254999999999</v>
+        <v>-4.4724254999999999</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -530,24 +685,838 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>160.7927</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>179.5908</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>194.6353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>206.6756</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>216.31180000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>224.02369999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>230.19579999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>235.1353</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>239.08860000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>242.25239999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>244.78450000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>246.81100000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>248.43279999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>249.73079999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>250.7696</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>251.601</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>252.2663</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>252.7988</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>253.22499999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>253.56610000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1">
+        <v>253.839</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>254.0575</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1">
+        <v>254.23230000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>254.37219999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1">
+        <v>254.48419999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1">
+        <v>254.57390000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1">
+        <v>254.6456</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1">
+        <v>254.703</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1">
+        <v>254.74889999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1">
+        <v>254.78569999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1">
+        <v>254.8151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1">
+        <v>254.83869999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1">
+        <v>254.85749999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1">
+        <v>254.87260000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1">
+        <v>254.88470000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1">
+        <v>254.89429999999999</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AK1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:37">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+      <c r="Z1">
+        <v>24</v>
+      </c>
+      <c r="AA1">
+        <v>25</v>
+      </c>
+      <c r="AB1">
+        <v>26</v>
+      </c>
+      <c r="AC1">
+        <v>27</v>
+      </c>
+      <c r="AD1">
+        <v>28</v>
+      </c>
+      <c r="AE1">
+        <v>29</v>
+      </c>
+      <c r="AF1">
+        <v>30</v>
+      </c>
+      <c r="AG1">
+        <v>31</v>
+      </c>
+      <c r="AH1">
+        <v>32</v>
+      </c>
+      <c r="AI1">
+        <v>33</v>
+      </c>
+      <c r="AJ1">
+        <v>34</v>
+      </c>
+      <c r="AK1">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>